<commit_message>
Added Context Menu to Export Calendar
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Infor\GrupoInvestigacion\4to\TransporteSerieNacionalFX\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\SNB-Biciam\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBC0CC1-9ED7-45DD-9489-39342B11B254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distancias entre las sedes" sheetId="1" r:id="rId1"/>
-    <sheet name="Localizaciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>PRI</t>
   </si>
@@ -121,26 +121,13 @@
   </si>
   <si>
     <t>Guantánamo</t>
-  </si>
-  <si>
-    <t>Occidental</t>
-  </si>
-  <si>
-    <t>Oriental</t>
-  </si>
-  <si>
-    <t>PED</t>
-  </si>
-  <si>
-    <t>Pedrito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,28 +143,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,16 +155,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF262626"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="63"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="63"/>
       </patternFill>
     </fill>
   </fills>
@@ -224,19 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,16 +499,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1464,69 +1413,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>